<commit_message>
Updating Intervention mechanism of action.xlsx
</commit_message>
<xml_diff>
--- a/Intervention mechanism/Intervention mechanism of action.xlsx
+++ b/Intervention mechanism/Intervention mechanism of action.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -565,32 +565,76 @@
           <t>process</t>
         </is>
       </c>
-      <c r="E2" s="2" t="inlineStr"/>
-      <c r="F2" s="2" t="inlineStr"/>
-      <c r="G2" s="2" t="inlineStr"/>
-      <c r="H2" s="2" t="inlineStr"/>
-      <c r="I2" s="2" t="inlineStr"/>
-      <c r="J2" s="2" t="inlineStr"/>
-      <c r="K2" s="2" t="inlineStr"/>
-      <c r="L2" s="2" t="inlineStr"/>
-      <c r="M2" s="2" t="inlineStr"/>
-      <c r="N2" s="2" t="inlineStr"/>
-      <c r="O2" s="2" t="inlineStr"/>
-      <c r="P2" s="2" t="inlineStr"/>
-      <c r="Q2" s="2" t="inlineStr"/>
-      <c r="R2" s="2" t="inlineStr"/>
+      <c r="E2" s="2" t="n"/>
+      <c r="F2" s="2" t="n"/>
+      <c r="G2" s="2" t="n"/>
+      <c r="H2" s="2" t="n"/>
+      <c r="I2" s="2" t="n"/>
+      <c r="J2" s="2" t="n"/>
+      <c r="K2" s="2" t="n"/>
+      <c r="L2" s="2" t="n"/>
+      <c r="M2" s="2" t="n"/>
+      <c r="N2" s="2" t="n"/>
+      <c r="O2" s="2" t="n"/>
+      <c r="P2" s="2" t="n"/>
+      <c r="Q2" s="2" t="n"/>
+      <c r="R2" s="2" t="n"/>
       <c r="S2" s="2" t="inlineStr">
         <is>
           <t>Proposed</t>
         </is>
       </c>
-      <c r="T2" s="2" t="inlineStr"/>
-      <c r="U2" s="2" t="inlineStr"/>
+      <c r="T2" s="2" t="n"/>
+      <c r="U2" s="2" t="n"/>
       <c r="V2" s="2" t="inlineStr">
         <is>
           <t>PS</t>
         </is>
       </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>BFO:0000015</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>process</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>p is a process = Def. p is an occurrent that has temporal proper parts and for some time t, p s-depends_on some material entity at t. (axiom label in BFO2 Reference: [083-003])</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>occurrent</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr"/>
+      <c r="F3" s="2" t="inlineStr"/>
+      <c r="G3" s="2" t="inlineStr"/>
+      <c r="H3" s="2" t="inlineStr"/>
+      <c r="I3" s="2" t="inlineStr"/>
+      <c r="J3" s="2" t="inlineStr"/>
+      <c r="K3" s="2" t="inlineStr"/>
+      <c r="L3" s="2" t="inlineStr"/>
+      <c r="M3" s="2" t="inlineStr"/>
+      <c r="N3" s="2" t="inlineStr"/>
+      <c r="O3" s="2" t="inlineStr"/>
+      <c r="P3" s="2" t="inlineStr"/>
+      <c r="Q3" s="2" t="inlineStr"/>
+      <c r="R3" s="2" t="inlineStr"/>
+      <c r="S3" s="2" t="inlineStr">
+        <is>
+          <t>Proposed</t>
+        </is>
+      </c>
+      <c r="T3" s="2" t="inlineStr"/>
+      <c r="U3" s="2" t="inlineStr"/>
+      <c r="V3" s="2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>